<commit_message>
Fonction de création de flotte completée, de destination e flotte, de test si il y a planete la ou le joueur clique.. bug de manufacture reglés. Doc updatée, notes pour Drago ajoutées
</commit_message>
<xml_diff>
--- a/doc/3-Galax_Scénarios_d'utilisation.xlsx
+++ b/doc/3-Galax_Scénarios_d'utilisation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="156" yWindow="132" windowWidth="18900" windowHeight="7836"/>
+    <workbookView xWindow="156" yWindow="192" windowWidth="18900" windowHeight="7776"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Humains</t>
   </si>
@@ -24,39 +24,15 @@
     <t>Machine</t>
   </si>
   <si>
-    <t>4- Humain se téléporte</t>
-  </si>
-  <si>
-    <t>5-Humain utilise le zappeur</t>
-  </si>
-  <si>
-    <t>6- Fin d'un niveau</t>
-  </si>
-  <si>
     <t>Scénarii d'utilisation</t>
   </si>
   <si>
-    <t>7- Fin de la partie</t>
-  </si>
-  <si>
-    <t>place des planètes</t>
-  </si>
-  <si>
     <t>détermine le nb de manufacture sur chaque planete</t>
   </si>
   <si>
-    <t>places les étoiles mères</t>
-  </si>
-  <si>
     <t>initialise les étoiles mères : 10 manufactures et 100 vaisseau par planete-mere</t>
   </si>
   <si>
-    <t>1-Faire une partie</t>
-  </si>
-  <si>
-    <t>humain joue son tour:</t>
-  </si>
-  <si>
     <t>clique sur une planete</t>
   </si>
   <si>
@@ -66,43 +42,127 @@
     <t>clique sur une destination</t>
   </si>
   <si>
-    <t>recommence au besoin jusqu'à qu'il clique sur GO</t>
-  </si>
-  <si>
-    <t>affiche les infos selon son niveau d'"intelligence"</t>
-  </si>
-  <si>
-    <t>ordi. Calculer la trajectoire et le temps en vertu de la distance</t>
-  </si>
-  <si>
-    <t>déplacement des Gubru selon leur stratégie d'essaiemement</t>
-  </si>
-  <si>
-    <t>(expansion vers l'extérieur a partir de leur étoile-mère)</t>
-  </si>
-  <si>
-    <t>déplacement des Czin selon leur strategie de déplacement (par grappes)</t>
-  </si>
-  <si>
     <t>Calcul de l'avancement des années par incrémentation de 0.1</t>
   </si>
   <si>
-    <t>à chaque incrémentation : on checke les déplacements</t>
-  </si>
-  <si>
-    <t>si combat il y a ,combat il y aura</t>
-  </si>
-  <si>
     <t>vérification si la partie est terminée</t>
   </si>
   <si>
     <t>Si oui : écran de fin de partie retour au menu</t>
   </si>
   <si>
-    <t>Sinon: on ajoute les vaisseaux selon les manufactures</t>
-  </si>
-  <si>
-    <t>On GOTO humain joue son tour</t>
+    <t>Calculer la trajectoire et le temps en vertu de la distance</t>
+  </si>
+  <si>
+    <t>1-Démarrer la partie</t>
+  </si>
+  <si>
+    <t>2-Préparer son tour</t>
+  </si>
+  <si>
+    <t>Vérifie que le nombre de vaisseau est plus grand que 0.</t>
+  </si>
+  <si>
+    <t>Vérifie qu'il a bien cliqué sur une étoile</t>
+  </si>
+  <si>
+    <t>3-Envoie de flotte</t>
+  </si>
+  <si>
+    <t>Enlever les vaisseaux de l'étoile en question</t>
+  </si>
+  <si>
+    <t>Inscrire la destination de la flotte</t>
+  </si>
+  <si>
+    <t>4- Exécuter le tour</t>
+  </si>
+  <si>
+    <t>à chaque incrémentation : on vérifie les déplacements</t>
+  </si>
+  <si>
+    <t>Création de la flotte</t>
+  </si>
+  <si>
+    <t>préparer des flotte selon leur force d'attaque</t>
+  </si>
+  <si>
+    <t>trouve une étoile proche</t>
+  </si>
+  <si>
+    <t>envoie des flottes</t>
+  </si>
+  <si>
+    <t>si c'est après une conquête, evalue le nombre de vaisseau de la flotte</t>
+  </si>
+  <si>
+    <t>si plus de 25 vaisseaux, laisser 15 vaisseaux et reoturne le reste a l'étoile-mère</t>
+  </si>
+  <si>
+    <t>Clique sur Go</t>
+  </si>
+  <si>
+    <t>5-Vérification de fin de partie</t>
+  </si>
+  <si>
+    <t>Ceci est fait pour chaque planête.</t>
+  </si>
+  <si>
+    <t>déplacement des Czin selon leur stratégie de "grappes"</t>
+  </si>
+  <si>
+    <t>Trouver une grappe</t>
+  </si>
+  <si>
+    <t>Prépare une armada</t>
+  </si>
+  <si>
+    <t>Envoie l'Armada sur la planete centrale de la grappe</t>
+  </si>
+  <si>
+    <t>Rassemble des forces sur cette étoile</t>
+  </si>
+  <si>
+    <t>Conquiert la grappe</t>
+  </si>
+  <si>
+    <t>Rassemble ses forces</t>
+  </si>
+  <si>
+    <t>Démarre une partie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> On effectue le combat</t>
+  </si>
+  <si>
+    <t>On inscrit les résultats du combat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinon: on ajoute les vaisseaux selon les manufactures </t>
+  </si>
+  <si>
+    <t>on redonne le tour au joueur</t>
+  </si>
+  <si>
+    <t>place des planètes aleatoirenment en vertu de la taille en x et y de l'univers</t>
+  </si>
+  <si>
+    <t>places les étoiles mères aléatoirement</t>
+  </si>
+  <si>
+    <t>Préparation des flottes des Gubru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si combat il y a , on évalue si le combat est surprise ou pas </t>
+  </si>
+  <si>
+    <t>Affiche les infos selon son niveau d'"intelligence"</t>
+  </si>
+  <si>
+    <t>Évalue si celle-ci est au joueur, si oui, on affiche le tout</t>
+  </si>
+  <si>
+    <t>Sinon, afficher les infos selon son niveau d'intelligence</t>
   </si>
 </sst>
 </file>
@@ -471,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +545,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -500,133 +560,241 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="14.55" x14ac:dyDescent="0.35"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="14.55" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>12</v>
+      <c r="A10" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>14</v>
+      <c r="C12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>16</v>
+      <c r="C14" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.55" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="C20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.55" x14ac:dyDescent="0.35">
-      <c r="C24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.55" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>6</v>
-      </c>
-    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" ht="14.55" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" ht="14.55" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>